<commit_message>
nba analysis file: analysis
</commit_message>
<xml_diff>
--- a/Glossary.xlsx
+++ b/Glossary.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nguye\Documents\TTU\5381\nba\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nguye\Documents\TTU\5381\nba\isqs5381_summer19nn\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2F7D9EC-2122-483D-95E8-2CF782552283}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{070D9AA4-E1B1-4E63-8082-E9E3477D4A99}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{D3189999-4818-444D-BCA3-F9A21EDF45E6}"/>
   </bookViews>
@@ -102,7 +102,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="148">
   <si>
     <r>
       <t>2P</t>
@@ -4102,7 +4102,7 @@
   <dimension ref="A1:C73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4291,9 +4291,6 @@
       <c r="B18" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C18" s="3" t="s">
-        <v>8</v>
-      </c>
     </row>
     <row r="19" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
@@ -4386,6 +4383,9 @@
       <c r="B28" s="2" t="s">
         <v>56</v>
       </c>
+      <c r="C28" s="3" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="29" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
@@ -4469,9 +4469,6 @@
       <c r="B38" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="C38" s="3" t="s">
-        <v>8</v>
-      </c>
     </row>
     <row r="39" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
@@ -4550,6 +4547,9 @@
       <c r="B47" s="2" t="s">
         <v>94</v>
       </c>
+      <c r="C47" s="3" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="48" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
@@ -4702,7 +4702,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="65" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>130</v>
       </c>
@@ -4710,7 +4710,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="66" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>132</v>
       </c>
@@ -4718,7 +4718,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="67" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>134</v>
       </c>
@@ -4726,7 +4726,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="68" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>136</v>
       </c>
@@ -4734,7 +4734,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="69" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>138</v>
       </c>
@@ -4742,15 +4742,18 @@
         <v>139</v>
       </c>
     </row>
-    <row r="70" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>140</v>
       </c>
       <c r="B70" s="2" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="71" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C70" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>142</v>
       </c>
@@ -4758,7 +4761,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="72" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>144</v>
       </c>
@@ -4766,7 +4769,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="73" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>146</v>
       </c>

</xml_diff>

<commit_message>
nba analysis file: vabs selected
</commit_message>
<xml_diff>
--- a/Glossary.xlsx
+++ b/Glossary.xlsx
@@ -8,83 +8,84 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nguye\Documents\TTU\5381\nba\isqs5381_summer19nn\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{070D9AA4-E1B1-4E63-8082-E9E3477D4A99}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE0ED807-BE7F-43F8-B6C1-BB4734569BCA}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{D3189999-4818-444D-BCA3-F9A21EDF45E6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{D3189999-4818-444D-BCA3-F9A21EDF45E6}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Glossary" sheetId="1" r:id="rId1"/>
+    <sheet name="Data Dictionary" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="age" localSheetId="0">Sheet1!$A$8</definedName>
-    <definedName name="ast" localSheetId="0">Sheet1!$A$9</definedName>
-    <definedName name="ast_pct" localSheetId="0">Sheet1!$A$10</definedName>
-    <definedName name="award_share" localSheetId="0">Sheet1!$A$11</definedName>
-    <definedName name="blk" localSheetId="0">Sheet1!$A$12</definedName>
-    <definedName name="blk_pct" localSheetId="0">Sheet1!$A$13</definedName>
-    <definedName name="bpm" localSheetId="0">Sheet1!$A$14</definedName>
-    <definedName name="def_rtg" localSheetId="0">Sheet1!$A$18</definedName>
-    <definedName name="dpoy" localSheetId="0">Sheet1!$A$15</definedName>
-    <definedName name="drb" localSheetId="0">Sheet1!$A$16</definedName>
-    <definedName name="drb_pct" localSheetId="0">Sheet1!$A$17</definedName>
-    <definedName name="dws" localSheetId="0">Sheet1!$A$19</definedName>
-    <definedName name="efg_pct" localSheetId="0">Sheet1!$A$20</definedName>
-    <definedName name="fg_pct" localSheetId="0">Sheet1!$A$22</definedName>
-    <definedName name="fg2_pct" localSheetId="0">Sheet1!$A$3</definedName>
-    <definedName name="fg2a" localSheetId="0">Sheet1!$A$4</definedName>
-    <definedName name="fg3_pct" localSheetId="0">Sheet1!$A$6</definedName>
-    <definedName name="fg3a" localSheetId="0">Sheet1!$A$7</definedName>
-    <definedName name="fga" localSheetId="0">Sheet1!$A$23</definedName>
-    <definedName name="four_factors" localSheetId="0">Sheet1!$A$27</definedName>
-    <definedName name="ft" localSheetId="0">Sheet1!$A$24</definedName>
-    <definedName name="ft_pct" localSheetId="0">Sheet1!$A$25</definedName>
-    <definedName name="fta" localSheetId="0">Sheet1!$A$26</definedName>
-    <definedName name="g" localSheetId="0">Sheet1!$A$28</definedName>
-    <definedName name="game_score" localSheetId="0">Sheet1!$A$30</definedName>
-    <definedName name="gb" localSheetId="0">Sheet1!$A$29</definedName>
-    <definedName name="gs" localSheetId="0">Sheet1!$A$31</definedName>
-    <definedName name="lg" localSheetId="0">Sheet1!$A$34</definedName>
-    <definedName name="losses" localSheetId="0">Sheet1!$A$32</definedName>
-    <definedName name="losses_pyth" localSheetId="0">Sheet1!$A$33</definedName>
-    <definedName name="mov" localSheetId="0">Sheet1!$A$37</definedName>
-    <definedName name="mp" localSheetId="0">Sheet1!$A$36</definedName>
-    <definedName name="mvp" localSheetId="0">Sheet1!$A$35</definedName>
-    <definedName name="off_rtg" localSheetId="0">Sheet1!$A$38</definedName>
-    <definedName name="opp_id" localSheetId="0">Sheet1!$A$39</definedName>
-    <definedName name="orb" localSheetId="0">Sheet1!$A$40</definedName>
-    <definedName name="orb_pct" localSheetId="0">Sheet1!$A$41</definedName>
-    <definedName name="ows" localSheetId="0">Sheet1!$A$42</definedName>
-    <definedName name="pace" localSheetId="0">Sheet1!$A$43</definedName>
-    <definedName name="per" localSheetId="0">Sheet1!$A$44</definedName>
-    <definedName name="per_36_mp" localSheetId="0">Sheet1!$A$45</definedName>
-    <definedName name="per_g" localSheetId="0">Sheet1!$A$46</definedName>
-    <definedName name="pf" localSheetId="0">Sheet1!$A$47</definedName>
-    <definedName name="poss" localSheetId="0">Sheet1!$A$48</definedName>
-    <definedName name="pprod" localSheetId="0">Sheet1!$A$49</definedName>
-    <definedName name="pts" localSheetId="0">Sheet1!$A$50</definedName>
-    <definedName name="roy" localSheetId="0">Sheet1!$A$51</definedName>
-    <definedName name="smoy" localSheetId="0">Sheet1!$A$52</definedName>
-    <definedName name="sos" localSheetId="0">Sheet1!$A$53</definedName>
-    <definedName name="srs" localSheetId="0">Sheet1!$A$54</definedName>
-    <definedName name="stl" localSheetId="0">Sheet1!$A$55</definedName>
-    <definedName name="stl_pct" localSheetId="0">Sheet1!$A$56</definedName>
-    <definedName name="stops" localSheetId="0">Sheet1!$A$57</definedName>
-    <definedName name="team" localSheetId="0">Sheet1!$A$58</definedName>
-    <definedName name="tov" localSheetId="0">Sheet1!$A$59</definedName>
-    <definedName name="tov_pct" localSheetId="0">Sheet1!$A$60</definedName>
-    <definedName name="trb" localSheetId="0">Sheet1!$A$61</definedName>
-    <definedName name="trb_pct" localSheetId="0">Sheet1!$A$62</definedName>
-    <definedName name="ts_pct" localSheetId="0">Sheet1!$A$63</definedName>
-    <definedName name="tsa" localSheetId="0">Sheet1!$A$64</definedName>
-    <definedName name="usg_pct" localSheetId="0">Sheet1!$A$65</definedName>
-    <definedName name="vorp" localSheetId="0">Sheet1!$A$66</definedName>
-    <definedName name="win_loss_pct" localSheetId="0">Sheet1!$A$69</definedName>
-    <definedName name="win_prob" localSheetId="0">Sheet1!$A$72</definedName>
-    <definedName name="wins" localSheetId="0">Sheet1!$A$67</definedName>
-    <definedName name="wins_pyth" localSheetId="0">Sheet1!$A$68</definedName>
-    <definedName name="ws" localSheetId="0">Sheet1!$A$70</definedName>
-    <definedName name="ws_per_48" localSheetId="0">Sheet1!$A$71</definedName>
-    <definedName name="year" localSheetId="0">Sheet1!$A$73</definedName>
+    <definedName name="age" localSheetId="0">Glossary!$A$8</definedName>
+    <definedName name="ast" localSheetId="0">Glossary!$A$9</definedName>
+    <definedName name="ast_pct" localSheetId="0">Glossary!$A$10</definedName>
+    <definedName name="award_share" localSheetId="0">Glossary!$A$11</definedName>
+    <definedName name="blk" localSheetId="0">Glossary!$A$12</definedName>
+    <definedName name="blk_pct" localSheetId="0">Glossary!$A$13</definedName>
+    <definedName name="bpm" localSheetId="0">Glossary!$A$14</definedName>
+    <definedName name="def_rtg" localSheetId="0">Glossary!$A$18</definedName>
+    <definedName name="dpoy" localSheetId="0">Glossary!$A$15</definedName>
+    <definedName name="drb" localSheetId="0">Glossary!$A$16</definedName>
+    <definedName name="drb_pct" localSheetId="0">Glossary!$A$17</definedName>
+    <definedName name="dws" localSheetId="0">Glossary!$A$19</definedName>
+    <definedName name="efg_pct" localSheetId="0">Glossary!$A$20</definedName>
+    <definedName name="fg_pct" localSheetId="0">Glossary!$A$22</definedName>
+    <definedName name="fg2_pct" localSheetId="0">Glossary!$A$3</definedName>
+    <definedName name="fg2a" localSheetId="0">Glossary!$A$4</definedName>
+    <definedName name="fg3_pct" localSheetId="0">Glossary!$A$6</definedName>
+    <definedName name="fg3a" localSheetId="0">Glossary!$A$7</definedName>
+    <definedName name="fga" localSheetId="0">Glossary!$A$23</definedName>
+    <definedName name="four_factors" localSheetId="0">Glossary!$A$27</definedName>
+    <definedName name="ft" localSheetId="0">Glossary!$A$24</definedName>
+    <definedName name="ft_pct" localSheetId="0">Glossary!$A$25</definedName>
+    <definedName name="fta" localSheetId="0">Glossary!$A$26</definedName>
+    <definedName name="g" localSheetId="0">Glossary!$A$28</definedName>
+    <definedName name="game_score" localSheetId="0">Glossary!$A$30</definedName>
+    <definedName name="gb" localSheetId="0">Glossary!$A$29</definedName>
+    <definedName name="gs" localSheetId="0">Glossary!$A$31</definedName>
+    <definedName name="lg" localSheetId="0">Glossary!$A$34</definedName>
+    <definedName name="losses" localSheetId="0">Glossary!$A$32</definedName>
+    <definedName name="losses_pyth" localSheetId="0">Glossary!$A$33</definedName>
+    <definedName name="mov" localSheetId="0">Glossary!$A$37</definedName>
+    <definedName name="mp" localSheetId="0">Glossary!$A$36</definedName>
+    <definedName name="mvp" localSheetId="0">Glossary!$A$35</definedName>
+    <definedName name="off_rtg" localSheetId="0">Glossary!$A$38</definedName>
+    <definedName name="opp_id" localSheetId="0">Glossary!$A$39</definedName>
+    <definedName name="orb" localSheetId="0">Glossary!$A$40</definedName>
+    <definedName name="orb_pct" localSheetId="0">Glossary!$A$41</definedName>
+    <definedName name="ows" localSheetId="0">Glossary!$A$42</definedName>
+    <definedName name="pace" localSheetId="0">Glossary!$A$43</definedName>
+    <definedName name="per" localSheetId="0">Glossary!$A$44</definedName>
+    <definedName name="per_36_mp" localSheetId="0">Glossary!$A$45</definedName>
+    <definedName name="per_g" localSheetId="0">Glossary!$A$46</definedName>
+    <definedName name="pf" localSheetId="0">Glossary!$A$47</definedName>
+    <definedName name="poss" localSheetId="0">Glossary!$A$48</definedName>
+    <definedName name="pprod" localSheetId="0">Glossary!$A$49</definedName>
+    <definedName name="pts" localSheetId="0">Glossary!$A$50</definedName>
+    <definedName name="roy" localSheetId="0">Glossary!$A$51</definedName>
+    <definedName name="smoy" localSheetId="0">Glossary!$A$52</definedName>
+    <definedName name="sos" localSheetId="0">Glossary!$A$53</definedName>
+    <definedName name="srs" localSheetId="0">Glossary!$A$54</definedName>
+    <definedName name="stl" localSheetId="0">Glossary!$A$55</definedName>
+    <definedName name="stl_pct" localSheetId="0">Glossary!$A$56</definedName>
+    <definedName name="stops" localSheetId="0">Glossary!$A$57</definedName>
+    <definedName name="team" localSheetId="0">Glossary!$A$58</definedName>
+    <definedName name="tov" localSheetId="0">Glossary!$A$59</definedName>
+    <definedName name="tov_pct" localSheetId="0">Glossary!$A$60</definedName>
+    <definedName name="trb" localSheetId="0">Glossary!$A$61</definedName>
+    <definedName name="trb_pct" localSheetId="0">Glossary!$A$62</definedName>
+    <definedName name="ts_pct" localSheetId="0">Glossary!$A$63</definedName>
+    <definedName name="tsa" localSheetId="0">Glossary!$A$64</definedName>
+    <definedName name="usg_pct" localSheetId="0">Glossary!$A$65</definedName>
+    <definedName name="vorp" localSheetId="0">Glossary!$A$66</definedName>
+    <definedName name="win_loss_pct" localSheetId="0">Glossary!$A$69</definedName>
+    <definedName name="win_prob" localSheetId="0">Glossary!$A$72</definedName>
+    <definedName name="wins" localSheetId="0">Glossary!$A$67</definedName>
+    <definedName name="wins_pyth" localSheetId="0">Glossary!$A$68</definedName>
+    <definedName name="ws" localSheetId="0">Glossary!$A$70</definedName>
+    <definedName name="ws_per_48" localSheetId="0">Glossary!$A$71</definedName>
+    <definedName name="year" localSheetId="0">Glossary!$A$73</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -102,7 +103,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1064" uniqueCount="159">
   <si>
     <r>
       <t>2P</t>
@@ -119,9 +120,6 @@
   </si>
   <si>
     <t>Description</t>
-  </si>
-  <si>
-    <t>Column_name</t>
   </si>
   <si>
     <t>2P%</t>
@@ -3015,9 +3013,6 @@
     </r>
   </si>
   <si>
-    <t>Use (X) - AllStar prediction</t>
-  </si>
-  <si>
     <r>
       <t>TSA</t>
     </r>
@@ -3666,6 +3661,45 @@
   </si>
   <si>
     <t> Year that the season occurred. Since the NBA season is split over two calendar years, the year given is the last year for that season. For example, the year for the 1999-00 season would be 2000.</t>
+  </si>
+  <si>
+    <t>Used for Modeling</t>
+  </si>
+  <si>
+    <t>Data Type</t>
+  </si>
+  <si>
+    <t>Variables</t>
+  </si>
+  <si>
+    <t>Player</t>
+  </si>
+  <si>
+    <t>Players names</t>
+  </si>
+  <si>
+    <t>Pos</t>
+  </si>
+  <si>
+    <t>Position</t>
+  </si>
+  <si>
+    <t>Assist percentage: an estimate of the percentage of teammate field goals a player assisted while he was on the floor.</t>
+  </si>
+  <si>
+    <t>Defensive Rebound Percentage: an estimate of the percentage of available defensive rebounds a player grabbed while he was on the floor</t>
+  </si>
+  <si>
+    <t>Offensive rebound percentage: an estimate of the percentage of available offensive rebounds a player grabbed while he was on the floor.</t>
+  </si>
+  <si>
+    <t>Block percentage: an estimate of the percentage of opponent two-point field goal attempts blocked by the player while he was on the floor.</t>
+  </si>
+  <si>
+    <t>Steal Percentage: an estimate of the percentage of opponent possessions that end with a steal by the player while he was on the floor.</t>
+  </si>
+  <si>
+    <t>Turnover percentage: an estimate of turnovers per 100 plays.</t>
   </si>
 </sst>
 </file>
@@ -3706,12 +3740,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -3726,18 +3766,65 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="8">
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -3791,12 +3878,26 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6D8B826B-A82F-4419-B190-B589CAC42EB4}" name="Table1" displayName="Table1" ref="A1:C73" totalsRowShown="0">
-  <autoFilter ref="A1:C73" xr:uid="{0D7E3112-6569-4BF7-9D7B-41815FD1FBFC}"/>
-  <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{79618815-BE60-41FB-B0F4-BDE65F9F3C31}" name="Column_name" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{9764C471-8D25-42E5-A03A-39ECC078F5E3}" name="Description" dataDxfId="1"/>
-    <tableColumn id="3" xr3:uid="{1C056923-5FD4-4C6F-8025-9206C700DC43}" name="Use (X) - AllStar prediction" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6D8B826B-A82F-4419-B190-B589CAC42EB4}" name="Table1" displayName="Table1" ref="A1:D73" totalsRowShown="0">
+  <autoFilter ref="A1:D73" xr:uid="{0D7E3112-6569-4BF7-9D7B-41815FD1FBFC}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{79618815-BE60-41FB-B0F4-BDE65F9F3C31}" name="Variables" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{9764C471-8D25-42E5-A03A-39ECC078F5E3}" name="Description" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{1C056923-5FD4-4C6F-8025-9206C700DC43}" name="Data Type" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{1933C082-F770-49FE-B385-B190C2891CF7}" name="Used for Modeling" dataDxfId="4"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{740B3279-E908-444C-BA34-7787B012C4E5}" name="Table13" displayName="Table13" ref="A1:D75" totalsRowShown="0">
+  <autoFilter ref="A1:D75" xr:uid="{3978729F-DD22-43A7-806E-496928F48D9D}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{D1BE4E05-D042-4EE5-AABD-7DFE804E9504}" name="Variables" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{26F6ED58-462D-4BB8-B9CE-4886DB2E63E5}" name="Description" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{9EE8A12E-2639-4F58-8A97-37CC3AA48937}" name="Data Type" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{516F29AF-7849-4860-87E0-1BB408D6BB26}" name="Used for Modeling" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4099,683 +4200,1559 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9F03A5B-3CF2-4D37-9AC2-830598C0CF5F}">
-  <dimension ref="A1:C73"/>
+  <dimension ref="A1:D73"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
     <col min="2" max="2" width="56.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="27.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>2</v>
+        <v>148</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+        <v>147</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="B4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="3"/>
+    </row>
+    <row r="5" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="B5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="3"/>
+    </row>
+    <row r="8" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" s="3"/>
+    </row>
+    <row r="12" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D14" s="3"/>
+    </row>
+    <row r="15" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D15" s="3"/>
+    </row>
+    <row r="16" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D18" s="3"/>
+    </row>
+    <row r="19" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D19" s="3"/>
+    </row>
+    <row r="20" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D20" s="3"/>
+    </row>
+    <row r="21" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D23" s="3"/>
+    </row>
+    <row r="24" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D26" s="3"/>
+    </row>
+    <row r="27" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D27" s="3"/>
+    </row>
+    <row r="28" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D29" s="3"/>
+    </row>
+    <row r="30" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D30" s="3"/>
+    </row>
+    <row r="31" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D31" s="3"/>
+    </row>
+    <row r="32" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D32" s="3"/>
+    </row>
+    <row r="33" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D33" s="3"/>
+    </row>
+    <row r="34" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D34" s="3"/>
+    </row>
+    <row r="35" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D35" s="3"/>
+    </row>
+    <row r="36" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D37" s="3"/>
+    </row>
+    <row r="38" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D38" s="3"/>
+    </row>
+    <row r="39" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D39" s="3"/>
+    </row>
+    <row r="40" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="D42" s="3"/>
+    </row>
+    <row r="43" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D43" s="3"/>
+    </row>
+    <row r="44" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D44" s="3"/>
+    </row>
+    <row r="45" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="D45" s="3"/>
+    </row>
+    <row r="46" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="D46" s="3"/>
+    </row>
+    <row r="47" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="D47" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D48" s="3"/>
+    </row>
+    <row r="49" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D49" s="3"/>
+    </row>
+    <row r="50" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D50" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D51" s="3"/>
+    </row>
+    <row r="52" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="D52" s="3"/>
+    </row>
+    <row r="53" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="D53" s="3"/>
+    </row>
+    <row r="54" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D54" s="3"/>
+    </row>
+    <row r="55" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="D55" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D56" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="D57" s="3"/>
+    </row>
+    <row r="58" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="D58" s="3"/>
+    </row>
+    <row r="59" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="D59" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="D60" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="D61" s="3"/>
+    </row>
+    <row r="62" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A62" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="D62" s="3"/>
+    </row>
+    <row r="63" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A63" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="D63" s="3"/>
+    </row>
+    <row r="64" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A64" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="D64" s="3"/>
+    </row>
+    <row r="65" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A65" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="D65" s="3"/>
+    </row>
+    <row r="66" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A66" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="D66" s="3"/>
+    </row>
+    <row r="67" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A67" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="D67" s="3"/>
+    </row>
+    <row r="68" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A68" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="D68" s="3"/>
+    </row>
+    <row r="69" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A69" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="D69" s="3"/>
+    </row>
+    <row r="70" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A70" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B70" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="D70" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A71" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="B71" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="D71" s="3"/>
+    </row>
+    <row r="72" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A72" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="D72" s="3"/>
+    </row>
+    <row r="73" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A73" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="D73" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF48700E-FA31-460E-90FE-FD787E818484}">
+  <dimension ref="A1:D75"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="255.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>148</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="3"/>
+      <c r="D3" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+    </row>
+    <row r="5" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="2" t="s">
+      <c r="B5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="2" t="s">
+    <row r="6" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="B6" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="C6" s="3"/>
+      <c r="D6" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+      <c r="B7" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+    </row>
+    <row r="8" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+      <c r="B8" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="C8" s="3"/>
+      <c r="D8" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+      <c r="B9" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="C9" s="3"/>
+      <c r="D9" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>19</v>
-      </c>
       <c r="B10" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+      <c r="B11" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+    </row>
+    <row r="12" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+      <c r="B12" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="C12" s="3"/>
+      <c r="D12" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C12" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>25</v>
-      </c>
       <c r="B13" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
+      <c r="B14" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+    </row>
+    <row r="15" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
+      <c r="B15" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+    </row>
+    <row r="16" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
+      <c r="B16" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="C16" s="3"/>
+      <c r="D16" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C16" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>33</v>
-      </c>
       <c r="B17" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C17" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
+      <c r="B18" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+    </row>
+    <row r="19" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
+      <c r="B19" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+    </row>
+    <row r="20" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
+      <c r="B20" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+    </row>
+    <row r="21" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
+      <c r="B21" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="C21" s="3"/>
+      <c r="D21" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A22" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="C21" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
+      <c r="B22" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="C22" s="3"/>
+      <c r="D22" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C22" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
+      <c r="B23" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+    </row>
+    <row r="24" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
+      <c r="B24" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="C24" s="3"/>
+      <c r="D24" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="C24" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
+      <c r="B25" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="C25" s="3"/>
+      <c r="D25" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C25" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
+      <c r="B26" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+    </row>
+    <row r="27" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="s">
+      <c r="B27" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+    </row>
+    <row r="28" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A28" s="4" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="s">
+      <c r="B28" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="C28" s="3"/>
+      <c r="D28" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C28" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
+      <c r="B29" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="C29" s="3"/>
+      <c r="D29" s="3"/>
+    </row>
+    <row r="30" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
+      <c r="B30" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="C30" s="3"/>
+      <c r="D30" s="3"/>
+    </row>
+    <row r="31" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A31" s="5" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
+      <c r="B31" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="C31" s="3"/>
+      <c r="D31" s="3"/>
+    </row>
+    <row r="32" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
+      <c r="B32" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="C32" s="3"/>
+      <c r="D32" s="3"/>
+    </row>
+    <row r="33" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
+      <c r="B33" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="B33" s="2" t="s">
+      <c r="C33" s="3"/>
+      <c r="D33" s="3"/>
+    </row>
+    <row r="34" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
+      <c r="B34" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="C34" s="3"/>
+      <c r="D34" s="3"/>
+    </row>
+    <row r="35" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A35" s="1" t="s">
+      <c r="B35" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="B35" s="2" t="s">
+      <c r="C35" s="3"/>
+      <c r="D35" s="3"/>
+    </row>
+    <row r="36" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A36" s="4" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A36" s="1" t="s">
+      <c r="B36" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="B36" s="2" t="s">
+      <c r="C36" s="3"/>
+      <c r="D36" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="C36" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A37" s="1" t="s">
+      <c r="B37" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="B37" s="2" t="s">
+      <c r="C37" s="3"/>
+      <c r="D37" s="3"/>
+    </row>
+    <row r="38" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A38" s="1" t="s">
+      <c r="B38" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="B38" s="2" t="s">
+      <c r="C38" s="3"/>
+      <c r="D38" s="3"/>
+    </row>
+    <row r="39" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A39" s="1" t="s">
+      <c r="B39" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="B39" s="2" t="s">
+      <c r="C39" s="3"/>
+      <c r="D39" s="3"/>
+    </row>
+    <row r="40" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A40" s="4" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A40" s="1" t="s">
+      <c r="B40" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="B40" s="2" t="s">
+      <c r="C40" s="3"/>
+      <c r="D40" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A41" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="C40" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A41" s="1" t="s">
-        <v>81</v>
-      </c>
       <c r="B41" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="C41" s="3"/>
+      <c r="D41" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="C41" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A42" s="1" t="s">
+      <c r="B42" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="B42" s="2" t="s">
+      <c r="C42" s="3"/>
+      <c r="D42" s="3"/>
+    </row>
+    <row r="43" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A43" s="1" t="s">
+      <c r="B43" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="B43" s="2" t="s">
+      <c r="C43" s="3"/>
+      <c r="D43" s="3"/>
+    </row>
+    <row r="44" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A44" s="5" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A44" s="1" t="s">
+      <c r="B44" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="B44" s="2" t="s">
+      <c r="C44" s="3"/>
+      <c r="D44" s="3"/>
+    </row>
+    <row r="45" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="45" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A45" s="1" t="s">
+      <c r="B45" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="B45" s="2" t="s">
+      <c r="C45" s="3"/>
+      <c r="D45" s="3"/>
+    </row>
+    <row r="46" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="46" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A46" s="1" t="s">
+      <c r="B46" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="B46" s="2" t="s">
+      <c r="C46" s="3"/>
+      <c r="D46" s="3"/>
+    </row>
+    <row r="47" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A47" s="4" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="47" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A47" s="1" t="s">
+      <c r="B47" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="B47" s="2" t="s">
+      <c r="C47" s="3"/>
+      <c r="D47" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="C47" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A48" s="1" t="s">
+      <c r="B48" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="B48" s="2" t="s">
+      <c r="C48" s="3"/>
+      <c r="D48" s="3"/>
+    </row>
+    <row r="49" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A49" s="1" t="s">
+      <c r="B49" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="B49" s="2" t="s">
+      <c r="C49" s="3"/>
+      <c r="D49" s="3"/>
+    </row>
+    <row r="50" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A50" s="4" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A50" s="1" t="s">
+      <c r="B50" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="B50" s="2" t="s">
+      <c r="C50" s="3"/>
+      <c r="D50" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="C50" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A51" s="1" t="s">
+      <c r="B51" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="B51" s="2" t="s">
+      <c r="C51" s="3"/>
+      <c r="D51" s="3"/>
+    </row>
+    <row r="52" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A52" s="1" t="s">
+      <c r="B52" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="B52" s="2" t="s">
+      <c r="C52" s="3"/>
+      <c r="D52" s="3"/>
+    </row>
+    <row r="53" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A53" s="1" t="s">
+      <c r="B53" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="B53" s="2" t="s">
+      <c r="C53" s="3"/>
+      <c r="D53" s="3"/>
+    </row>
+    <row r="54" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A54" s="1" t="s">
+      <c r="B54" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="B54" s="2" t="s">
+      <c r="C54" s="3"/>
+      <c r="D54" s="3"/>
+    </row>
+    <row r="55" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A55" s="4" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="55" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A55" s="1" t="s">
+      <c r="B55" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="B55" s="2" t="s">
+      <c r="C55" s="3"/>
+      <c r="D55" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A56" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="C55" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A56" s="1" t="s">
-        <v>111</v>
-      </c>
       <c r="B56" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="C56" s="3"/>
+      <c r="D56" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="C56" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A57" s="1" t="s">
+      <c r="B57" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="B57" s="2" t="s">
+      <c r="C57" s="3"/>
+      <c r="D57" s="3"/>
+    </row>
+    <row r="58" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A58" s="4" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="58" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A58" s="1" t="s">
+      <c r="B58" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="B58" s="2" t="s">
+      <c r="C58" s="3"/>
+      <c r="D58" s="3"/>
+    </row>
+    <row r="59" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A59" s="4" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="59" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A59" s="1" t="s">
+      <c r="B59" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="B59" s="2" t="s">
+      <c r="C59" s="3"/>
+      <c r="D59" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A60" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="C59" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A60" s="1" t="s">
-        <v>119</v>
-      </c>
       <c r="B60" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="C60" s="3"/>
+      <c r="D60" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="C60" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A61" s="1" t="s">
+      <c r="B61" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="B61" s="2" t="s">
+      <c r="C61" s="3"/>
+      <c r="D61" s="3"/>
+    </row>
+    <row r="62" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A62" s="1" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="62" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A62" s="1" t="s">
+      <c r="B62" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="B62" s="2" t="s">
+      <c r="C62" s="3"/>
+      <c r="D62" s="3"/>
+    </row>
+    <row r="63" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A63" s="5" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="63" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A63" s="1" t="s">
+      <c r="B63" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="B63" s="2" t="s">
+      <c r="C63" s="3"/>
+      <c r="D63" s="3"/>
+    </row>
+    <row r="64" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A64" s="1" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="64" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A64" s="1" t="s">
+      <c r="B64" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="C64" s="3"/>
+      <c r="D64" s="3"/>
+    </row>
+    <row r="65" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A65" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="B64" s="2" t="s">
+      <c r="B65" s="2" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="65" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A65" s="1" t="s">
+      <c r="C65" s="3"/>
+      <c r="D65" s="3"/>
+    </row>
+    <row r="66" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A66" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="B65" s="2" t="s">
+      <c r="B66" s="2" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="66" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A66" s="1" t="s">
+      <c r="C66" s="3"/>
+      <c r="D66" s="3"/>
+    </row>
+    <row r="67" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A67" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="B66" s="2" t="s">
+      <c r="B67" s="2" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="67" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A67" s="1" t="s">
+      <c r="C67" s="3"/>
+      <c r="D67" s="3"/>
+    </row>
+    <row r="68" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A68" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="B67" s="2" t="s">
+      <c r="B68" s="2" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="68" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A68" s="1" t="s">
+      <c r="C68" s="3"/>
+      <c r="D68" s="3"/>
+    </row>
+    <row r="69" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A69" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="B68" s="2" t="s">
+      <c r="B69" s="2" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="69" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A69" s="1" t="s">
+      <c r="C69" s="3"/>
+      <c r="D69" s="3"/>
+    </row>
+    <row r="70" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A70" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="B69" s="2" t="s">
+      <c r="B70" s="2" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="70" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A70" s="1" t="s">
+      <c r="C70" s="3"/>
+      <c r="D70" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A71" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="B70" s="2" t="s">
+      <c r="B71" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="C70" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A71" s="1" t="s">
+      <c r="C71" s="3"/>
+      <c r="D71" s="3"/>
+    </row>
+    <row r="72" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A72" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="B71" s="2" t="s">
+      <c r="B72" s="2" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="72" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A72" s="1" t="s">
+      <c r="C72" s="3"/>
+      <c r="D72" s="3"/>
+    </row>
+    <row r="73" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A73" s="4" t="s">
         <v>144</v>
       </c>
-      <c r="B72" s="2" t="s">
+      <c r="B73" s="2" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="73" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A73" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="B73" s="2" t="s">
-        <v>147</v>
-      </c>
+      <c r="C73" s="3"/>
+      <c r="D73" s="3"/>
+    </row>
+    <row r="74" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A74" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="C74" s="3"/>
+      <c r="D74" s="3"/>
+    </row>
+    <row r="75" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A75" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="B75" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="C75" s="3"/>
+      <c r="D75" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
nba analysis file: code updated
</commit_message>
<xml_diff>
--- a/Glossary.xlsx
+++ b/Glossary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nguye\Documents\TTU\5381\nba\isqs5381_summer19nn\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE0ED807-BE7F-43F8-B6C1-BB4734569BCA}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0590D0F3-A7F7-4640-90A8-344C6AEE3A0B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{D3189999-4818-444D-BCA3-F9A21EDF45E6}"/>
   </bookViews>
@@ -103,7 +103,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1064" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="159">
   <si>
     <r>
       <t>2P</t>
@@ -3779,7 +3779,15 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="9">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FF000000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -3881,10 +3889,10 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6D8B826B-A82F-4419-B190-B589CAC42EB4}" name="Table1" displayName="Table1" ref="A1:D73" totalsRowShown="0">
   <autoFilter ref="A1:D73" xr:uid="{0D7E3112-6569-4BF7-9D7B-41815FD1FBFC}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{79618815-BE60-41FB-B0F4-BDE65F9F3C31}" name="Variables" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{9764C471-8D25-42E5-A03A-39ECC078F5E3}" name="Description" dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{1C056923-5FD4-4C6F-8025-9206C700DC43}" name="Data Type" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{1933C082-F770-49FE-B385-B190C2891CF7}" name="Used for Modeling" dataDxfId="4"/>
+    <tableColumn id="1" xr3:uid="{79618815-BE60-41FB-B0F4-BDE65F9F3C31}" name="Variables" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{9764C471-8D25-42E5-A03A-39ECC078F5E3}" name="Description" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{1C056923-5FD4-4C6F-8025-9206C700DC43}" name="Data Type" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{1933C082-F770-49FE-B385-B190C2891CF7}" name="Used for Modeling" dataDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3892,12 +3900,16 @@
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{740B3279-E908-444C-BA34-7787B012C4E5}" name="Table13" displayName="Table13" ref="A1:D75" totalsRowShown="0">
-  <autoFilter ref="A1:D75" xr:uid="{3978729F-DD22-43A7-806E-496928F48D9D}"/>
+  <autoFilter ref="A1:D75" xr:uid="{3978729F-DD22-43A7-806E-496928F48D9D}">
+    <filterColumn colId="0">
+      <colorFilter dxfId="0"/>
+    </filterColumn>
+  </autoFilter>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{D1BE4E05-D042-4EE5-AABD-7DFE804E9504}" name="Variables" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{26F6ED58-462D-4BB8-B9CE-4886DB2E63E5}" name="Description" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{9EE8A12E-2639-4F58-8A97-37CC3AA48937}" name="Data Type" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{516F29AF-7849-4860-87E0-1BB408D6BB26}" name="Used for Modeling" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{D1BE4E05-D042-4EE5-AABD-7DFE804E9504}" name="Variables" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{26F6ED58-462D-4BB8-B9CE-4886DB2E63E5}" name="Description" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{9EE8A12E-2639-4F58-8A97-37CC3AA48937}" name="Data Type" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{516F29AF-7849-4860-87E0-1BB408D6BB26}" name="Used for Modeling" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4938,14 +4950,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF48700E-FA31-460E-90FE-FD787E818484}">
   <dimension ref="A1:D75"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="255.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -4986,7 +4997,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -5020,7 +5031,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
@@ -5066,7 +5077,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>20</v>
       </c>
@@ -5100,7 +5111,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>26</v>
       </c>
@@ -5110,7 +5121,7 @@
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
     </row>
-    <row r="15" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>28</v>
       </c>
@@ -5144,7 +5155,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>34</v>
       </c>
@@ -5154,7 +5165,7 @@
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
     </row>
-    <row r="19" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>36</v>
       </c>
@@ -5164,7 +5175,7 @@
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
     </row>
-    <row r="20" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>38</v>
       </c>
@@ -5198,7 +5209,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>44</v>
       </c>
@@ -5232,7 +5243,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>50</v>
       </c>
@@ -5242,7 +5253,7 @@
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
     </row>
-    <row r="27" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>52</v>
       </c>
@@ -5264,7 +5275,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>56</v>
       </c>
@@ -5274,7 +5285,7 @@
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
     </row>
-    <row r="30" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>58</v>
       </c>
@@ -5284,7 +5295,7 @@
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
     </row>
-    <row r="31" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
         <v>60</v>
       </c>
@@ -5294,7 +5305,7 @@
       <c r="C31" s="3"/>
       <c r="D31" s="3"/>
     </row>
-    <row r="32" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>62</v>
       </c>
@@ -5304,7 +5315,7 @@
       <c r="C32" s="3"/>
       <c r="D32" s="3"/>
     </row>
-    <row r="33" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>64</v>
       </c>
@@ -5314,7 +5325,7 @@
       <c r="C33" s="3"/>
       <c r="D33" s="3"/>
     </row>
-    <row r="34" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>66</v>
       </c>
@@ -5324,7 +5335,7 @@
       <c r="C34" s="3"/>
       <c r="D34" s="3"/>
     </row>
-    <row r="35" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>68</v>
       </c>
@@ -5346,7 +5357,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>72</v>
       </c>
@@ -5356,7 +5367,7 @@
       <c r="C37" s="3"/>
       <c r="D37" s="3"/>
     </row>
-    <row r="38" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>74</v>
       </c>
@@ -5366,7 +5377,7 @@
       <c r="C38" s="3"/>
       <c r="D38" s="3"/>
     </row>
-    <row r="39" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>76</v>
       </c>
@@ -5400,7 +5411,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>82</v>
       </c>
@@ -5410,7 +5421,7 @@
       <c r="C42" s="3"/>
       <c r="D42" s="3"/>
     </row>
-    <row r="43" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>84</v>
       </c>
@@ -5420,7 +5431,7 @@
       <c r="C43" s="3"/>
       <c r="D43" s="3"/>
     </row>
-    <row r="44" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
         <v>86</v>
       </c>
@@ -5430,7 +5441,7 @@
       <c r="C44" s="3"/>
       <c r="D44" s="3"/>
     </row>
-    <row r="45" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>88</v>
       </c>
@@ -5440,7 +5451,7 @@
       <c r="C45" s="3"/>
       <c r="D45" s="3"/>
     </row>
-    <row r="46" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>90</v>
       </c>
@@ -5462,7 +5473,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>94</v>
       </c>
@@ -5472,7 +5483,7 @@
       <c r="C48" s="3"/>
       <c r="D48" s="3"/>
     </row>
-    <row r="49" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>96</v>
       </c>
@@ -5494,7 +5505,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>100</v>
       </c>
@@ -5504,7 +5515,7 @@
       <c r="C51" s="3"/>
       <c r="D51" s="3"/>
     </row>
-    <row r="52" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>102</v>
       </c>
@@ -5514,7 +5525,7 @@
       <c r="C52" s="3"/>
       <c r="D52" s="3"/>
     </row>
-    <row r="53" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>104</v>
       </c>
@@ -5524,7 +5535,7 @@
       <c r="C53" s="3"/>
       <c r="D53" s="3"/>
     </row>
-    <row r="54" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>106</v>
       </c>
@@ -5558,7 +5569,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="57" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>112</v>
       </c>
@@ -5602,7 +5613,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="61" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>120</v>
       </c>
@@ -5612,7 +5623,7 @@
       <c r="C61" s="3"/>
       <c r="D61" s="3"/>
     </row>
-    <row r="62" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>122</v>
       </c>
@@ -5622,7 +5633,7 @@
       <c r="C62" s="3"/>
       <c r="D62" s="3"/>
     </row>
-    <row r="63" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" s="5" t="s">
         <v>124</v>
       </c>
@@ -5632,7 +5643,7 @@
       <c r="C63" s="3"/>
       <c r="D63" s="3"/>
     </row>
-    <row r="64" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>126</v>
       </c>
@@ -5642,7 +5653,7 @@
       <c r="C64" s="3"/>
       <c r="D64" s="3"/>
     </row>
-    <row r="65" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>128</v>
       </c>
@@ -5652,7 +5663,7 @@
       <c r="C65" s="3"/>
       <c r="D65" s="3"/>
     </row>
-    <row r="66" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>130</v>
       </c>
@@ -5662,7 +5673,7 @@
       <c r="C66" s="3"/>
       <c r="D66" s="3"/>
     </row>
-    <row r="67" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" s="5" t="s">
         <v>132</v>
       </c>
@@ -5672,7 +5683,7 @@
       <c r="C67" s="3"/>
       <c r="D67" s="3"/>
     </row>
-    <row r="68" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>134</v>
       </c>
@@ -5682,7 +5693,7 @@
       <c r="C68" s="3"/>
       <c r="D68" s="3"/>
     </row>
-    <row r="69" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>136</v>
       </c>
@@ -5704,7 +5715,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="71" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>140</v>
       </c>
@@ -5714,7 +5725,7 @@
       <c r="C71" s="3"/>
       <c r="D71" s="3"/>
     </row>
-    <row r="72" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>142</v>
       </c>

</xml_diff>